<commit_message>
Rajout des cartes dimension qui avait disparu !
Ambre
</commit_message>
<xml_diff>
--- a/projet.xlsx
+++ b/projet.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\projet\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD978062-13BA-4400-8F99-6AE057E9CC9D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{85D5CD69-D5C1-4550-A07E-D389683ECBE5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19350" windowHeight="7740" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -19,9 +13,9 @@
     <sheet name="Feuil4" sheetId="4" r:id="rId4"/>
     <sheet name="Feuil5" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -35,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="143">
   <si>
     <t>date</t>
   </si>
@@ -91,9 +85,6 @@
     <t>Usage</t>
   </si>
   <si>
-    <t>personnage1</t>
-  </si>
-  <si>
     <t>joueur 1</t>
   </si>
   <si>
@@ -461,13 +452,19 @@
   </si>
   <si>
     <t>{Mohamed-Aurélie-Frederic-Agathe-Elise}</t>
+  </si>
+  <si>
+    <t>PARTIE 1</t>
+  </si>
+  <si>
+    <t>USAGE1 (PERSONNAGE 1)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -535,9 +532,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -552,6 +546,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -614,7 +611,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -666,7 +663,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -860,27 +857,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9ABCDEA-9505-49AA-AF5A-D2E6BACE4251}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="17.5703125" customWidth="1"/>
     <col min="4" max="4" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -894,8 +891,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="7">
+    <row r="4" spans="2:5">
+      <c r="B4" s="6">
         <v>1</v>
       </c>
       <c r="C4" s="3">
@@ -908,51 +905,51 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5">
       <c r="B5" s="5">
         <v>2</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5">
       <c r="B6" s="5">
         <v>3</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5">
       <c r="B7" s="5">
         <v>4</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" location="Feuil2!A1" display="Feuil2!A1" xr:uid="{54F11131-3815-4FD8-AD62-09E1218A0D6C}"/>
+    <hyperlink ref="B4" location="Feuil2!A1" display="Feuil2!A1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -960,19 +957,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8788094B-1454-4218-B4CA-0BB94054F8B4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C2:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="4" max="4" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:7">
       <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
@@ -989,125 +984,125 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C3" s="7">
+    <row r="3" spans="3:7">
+      <c r="C3" s="6">
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E3" s="2">
         <v>20</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="3:7">
       <c r="C4" s="2">
         <v>2</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E4" s="2">
         <v>20</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="3:7">
       <c r="C5" s="2">
         <v>3</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E5" s="2">
         <v>20</v>
       </c>
       <c r="F5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="3:7">
       <c r="C6" s="2">
         <v>4</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E6" s="2">
         <v>20</v>
       </c>
       <c r="F6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="3:7">
       <c r="C7" s="2">
         <v>5</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E7" s="2">
         <v>20</v>
       </c>
       <c r="F7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="3:7">
       <c r="C8" s="2">
         <v>6</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E8" s="2">
         <v>20</v>
       </c>
       <c r="F8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" location="Feuil3!A1" display="Feuil3!A1" xr:uid="{15B4A038-B09D-48F2-90E5-36F52B5540E6}"/>
+    <hyperlink ref="C3" location="Feuil3!A1" display="Feuil3!A1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8171F86F-85B5-4744-A991-8FD360D0B777}">
-  <dimension ref="C2:I8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="12.7109375" customWidth="1"/>
     <col min="3" max="3" width="21.7109375" customWidth="1"/>
@@ -1118,7 +1113,10 @@
     <col min="8" max="8" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>141</v>
+      </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -1127,147 +1125,147 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="3:9" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="10" t="s">
+    <row r="3" spans="1:9" ht="95.25" customHeight="1">
+      <c r="C3" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="F3" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="92.25" customHeight="1">
+      <c r="C4" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="90">
+      <c r="C5" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="90">
+      <c r="C6" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="90">
+      <c r="C7" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="90">
+      <c r="C8" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="3:9" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="3:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="C5" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="3:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="C6" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="3:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="C7" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E7" s="8" t="s">
+      <c r="E8" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="I8" s="7" t="s">
         <v>57</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="3:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="C8" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" location="Feuil4!A1" display="locomotion : Ailes" xr:uid="{A4B0F9C1-B93A-4D87-A464-72DD4F32C393}"/>
+    <hyperlink ref="C3" location="Feuil4!A1" display="locomotion : Ailes"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1275,14 +1273,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F855C673-4BDE-4DAA-8745-0EFC45C8434E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:J23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="19.7109375" customWidth="1"/>
     <col min="4" max="4" width="19.5703125" customWidth="1"/>
@@ -1293,8 +1289,8 @@
     <col min="10" max="10" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="11" t="s">
+    <row r="2" spans="2:10">
+      <c r="B2" s="10" t="s">
         <v>14</v>
       </c>
       <c r="C2" s="1"/>
@@ -1302,528 +1298,530 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="2:10" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" ht="58.5" customHeight="1">
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="E3" s="8" t="s">
+      <c r="C3" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>13</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" ht="43.5" customHeight="1">
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>78</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>79</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="I4" s="8" t="s">
+      <c r="H4" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="I4" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="J4" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" ht="45">
       <c r="B5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="E5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="I5" s="8" t="s">
+      <c r="H5" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="J5" s="8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="I5" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" ht="45">
       <c r="B6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="E6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>13</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="J6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="J6" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" ht="45">
       <c r="B7" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>79</v>
+        <v>69</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>78</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="H7" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="I7" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="I7" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="J7" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10">
       <c r="B10" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="G10" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" ht="45">
       <c r="B11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>79</v>
+        <v>18</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>78</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="I11" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="J11" s="8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" ht="45">
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="D12" s="8" t="s">
+      <c r="C12" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="E12" s="8" t="s">
-        <v>79</v>
+      <c r="D12" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>78</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H12" s="8" t="s">
+      <c r="H12" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="I12" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="I12" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="J12" s="8" t="s">
+      <c r="J12" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" ht="45">
       <c r="B13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="E13" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>13</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H13" s="8" t="s">
+      <c r="H13" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="I13" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="I13" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="J13" s="8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="J13" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" ht="45">
       <c r="B14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" ht="30">
+      <c r="B15" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="D14" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H14" s="8" t="s">
+      <c r="D15" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="I15" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="I14" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="J14" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="H15" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="I15" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="J15" s="8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="J15" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10">
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+    </row>
+    <row r="18" spans="2:10">
       <c r="B18" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="G18" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
     </row>
-    <row r="19" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" ht="45">
       <c r="B19" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>79</v>
+        <v>18</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>78</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H19" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="I19" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="J19" s="8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="J19" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" ht="45">
       <c r="B20" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="E20" s="8" t="s">
+      <c r="C20" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E20" s="7" t="s">
         <v>13</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H20" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="I20" s="8" t="s">
+      <c r="H20" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="J20" s="8" t="s">
+      <c r="I20" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="J20" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10" ht="30">
       <c r="B21" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="E21" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="E21" s="7" t="s">
         <v>13</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H21" s="8" t="s">
+      <c r="H21" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" ht="30">
+      <c r="B22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="I22" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="I21" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="J21" s="8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B22" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="8" t="s">
+      <c r="J22" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" ht="30">
+      <c r="B23" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C23" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="D22" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G22" s="1" t="s">
+      <c r="D23" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H22" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="I22" s="8" t="s">
+      <c r="H23" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="I23" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="J22" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="23" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B23" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H23" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="I23" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="J23" s="8" t="s">
+      <c r="J23" s="7" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" location="Feuil5!A1" display="Usage 1" xr:uid="{BAFF30C6-9A59-425E-BC24-13F0F83FE973}"/>
+    <hyperlink ref="B2" location="Feuil5!A1" display="Usage 1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5AE1F27-16A9-437C-9C16-DF9D507AA6A1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:16">
       <c r="B3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="C3" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6" t="s">
+      <c r="D3" s="11"/>
+      <c r="E3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6" t="s">
+      <c r="F3" s="11"/>
+      <c r="G3" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="6"/>
+      <c r="H3" s="11"/>
       <c r="J3" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="K3" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="K3" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6" t="s">
+      <c r="L3" s="11"/>
+      <c r="M3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6" t="s">
+      <c r="N3" s="11"/>
+      <c r="O3" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="P3" s="6"/>
-    </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="P3" s="11"/>
+    </row>
+    <row r="4" spans="2:16">
       <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
       <c r="J4" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
       <c r="N4" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:16">
       <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
@@ -1835,153 +1833,153 @@
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
       <c r="N5" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:16">
       <c r="B6" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H6" s="4"/>
       <c r="J6" s="4" t="s">
         <v>5</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
       <c r="O6" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="P6" s="4"/>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:16">
       <c r="B7" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="J7" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L7" s="4"/>
       <c r="M7" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N7" s="4"/>
       <c r="O7" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="P7" s="4"/>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:16">
       <c r="B8" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="J8" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L8" s="4"/>
       <c r="M8" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N8" s="4"/>
       <c r="O8" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="P8" s="4"/>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:16">
       <c r="B11" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C11" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6" t="s">
+      <c r="D11" s="11"/>
+      <c r="E11" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6" t="s">
+      <c r="F11" s="11"/>
+      <c r="G11" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="6"/>
+      <c r="H11" s="11"/>
       <c r="J11" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="K11" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="K11" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6" t="s">
+      <c r="L11" s="11"/>
+      <c r="M11" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6" t="s">
+      <c r="N11" s="11"/>
+      <c r="O11" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="P11" s="6"/>
-    </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="P11" s="11"/>
+    </row>
+    <row r="12" spans="2:16">
       <c r="B12" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L12" s="4"/>
       <c r="M12" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:16">
       <c r="B13" s="4" t="s">
         <v>5</v>
       </c>
@@ -2000,166 +1998,166 @@
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:16">
       <c r="B14" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J14" s="4" t="s">
         <v>5</v>
       </c>
       <c r="K14" s="4"/>
       <c r="L14" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M14" s="4"/>
       <c r="N14" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O14" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="P14" s="4"/>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:16">
       <c r="B15" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
       <c r="J15" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K15" s="4"/>
       <c r="L15" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M15" s="4"/>
       <c r="N15" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:16">
       <c r="B16" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G16" s="4"/>
       <c r="H16" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L16" s="4"/>
       <c r="M16" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
     </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:16">
       <c r="B20" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C20" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6" t="s">
+      <c r="D20" s="11"/>
+      <c r="E20" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6" t="s">
+      <c r="F20" s="11"/>
+      <c r="G20" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="H20" s="6"/>
+      <c r="H20" s="11"/>
       <c r="J20" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="K20" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="K20" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6" t="s">
+      <c r="L20" s="11"/>
+      <c r="M20" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="N20" s="6"/>
-      <c r="O20" s="6" t="s">
+      <c r="N20" s="11"/>
+      <c r="O20" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="P20" s="6"/>
-    </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="P20" s="11"/>
+    </row>
+    <row r="21" spans="2:16">
       <c r="B21" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H21" s="4"/>
       <c r="J21" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
       <c r="O21" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P21" s="4"/>
     </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:16">
       <c r="B22" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
@@ -2170,116 +2168,116 @@
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
       <c r="M22" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
     </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:16">
       <c r="B23" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H23" s="4"/>
       <c r="J23" s="4" t="s">
         <v>5</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L23" s="4"/>
       <c r="M23" s="4"/>
       <c r="N23" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O23" s="4"/>
       <c r="P23" s="4"/>
     </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:16">
       <c r="B24" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F24" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>24</v>
       </c>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
       <c r="J24" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
       <c r="M24" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N24" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O24" s="4"/>
       <c r="P24" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16">
       <c r="B25" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
       <c r="J25" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
       <c r="N25" s="4"/>
       <c r="O25" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P25" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="O11:P11"/>
     <mergeCell ref="O20:P20"/>
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="G20:H20"/>
     <mergeCell ref="K20:L20"/>
     <mergeCell ref="M20:N20"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="G11:H11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>